<commit_message>
Added replaced values with mean values for each feature
</commit_message>
<xml_diff>
--- a/finalProject/resultados.xlsx
+++ b/finalProject/resultados.xlsx
@@ -68,10 +68,10 @@
     <t>Primary Type, Location Description, Domestic, Latitude, Longitude, month, day, Period_MORNING, Period_DAY</t>
   </si>
   <si>
-    <t>Only Locations</t>
+    <t>KNN K = x variation</t>
   </si>
   <si>
-    <t>KNN K = x variation</t>
+    <t>Only Locations THEFTandBATTERY</t>
   </si>
 </sst>
 </file>
@@ -331,7 +331,7 @@
                   <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,7 +412,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Only Locations</c:v>
+                  <c:v>Only Locations THEFTandBATTERY</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1213,16 +1213,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1321,6 +1321,94 @@
         <a:xfrm>
           <a:off x="4800600" y="6565900"/>
           <a:ext cx="3784600" cy="2621624"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>108942</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="552450" y="9334500"/>
+          <a:ext cx="3695699" cy="2560042"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>179996</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>431799</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4853596" y="9309100"/>
+          <a:ext cx="3795103" cy="2628900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1597,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1661,7 +1749,7 @@
         <v>0.53</v>
       </c>
       <c r="E4">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1683,7 +1771,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>0.57999999999999996</v>
@@ -1716,7 +1804,7 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added results with xgboost
</commit_message>
<xml_diff>
--- a/finalProject/resultados.xlsx
+++ b/finalProject/resultados.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Resultados </t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Only Locations THEFTandBATTERY</t>
+  </si>
+  <si>
+    <t>HOMICIDEandMOTORTHEFTandNARCOTICS</t>
+  </si>
+  <si>
+    <t>XGBOOST</t>
   </si>
 </sst>
 </file>
@@ -231,9 +237,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$E$2</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Naive Bayes</c:v>
                 </c:pt>
@@ -245,16 +251,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>XGBOOST</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$E$3</c:f>
+              <c:f>Sheet1!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.16</c:v>
                 </c:pt>
@@ -266,6 +275,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -297,9 +309,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$E$2</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Naive Bayes</c:v>
                 </c:pt>
@@ -311,16 +323,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>XGBOOST</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$E$4</c:f>
+              <c:f>Sheet1!$B$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.74</c:v>
                 </c:pt>
@@ -331,6 +346,9 @@
                   <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -363,9 +381,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$E$2</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Naive Bayes</c:v>
                 </c:pt>
@@ -377,16 +395,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>XGBOOST</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$E$5</c:f>
+              <c:f>Sheet1!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.64</c:v>
                 </c:pt>
@@ -398,6 +419,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -429,9 +453,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$E$2</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Naive Bayes</c:v>
                 </c:pt>
@@ -443,16 +467,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>XGBOOST</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$E$6</c:f>
+              <c:f>Sheet1!$B$6:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0.58</c:v>
                 </c:pt>
@@ -464,6 +491,81 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HOMICIDEandMOTORTHEFTandNARCOTICS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>KNN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GMM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>XGBOOST</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1249,8 +1351,8 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>416904</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>302604</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1337,8 +1439,8 @@
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>108942</xdr:rowOff>
     </xdr:to>
@@ -1683,25 +1785,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1717,8 +1819,11 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1734,8 +1839,11 @@
       <c r="E3">
         <v>0.36</v>
       </c>
+      <c r="F3">
+        <v>0.37</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1751,8 +1859,11 @@
       <c r="E4">
         <v>0.8</v>
       </c>
+      <c r="F4">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1768,8 +1879,11 @@
       <c r="E5">
         <v>0.67</v>
       </c>
+      <c r="F5">
+        <v>0.68</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1785,8 +1899,31 @@
       <c r="E6">
         <v>0.66</v>
       </c>
+      <c r="F6">
+        <v>0.65</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0.54</v>
+      </c>
+      <c r="C7">
+        <v>0.73</v>
+      </c>
+      <c r="D7">
+        <v>0.41</v>
+      </c>
+      <c r="E7">
+        <v>0.76</v>
+      </c>
+      <c r="F7">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1794,7 +1931,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>

</xml_diff>